<commit_message>
updated team member report
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
+++ b/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
@@ -947,12 +947,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -962,9 +959,12 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1099,7 +1099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -1421,6 +1421,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -1430,15 +1439,6 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1578,7 +1578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -1900,12 +1900,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -1918,6 +1912,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2367,12 +2367,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2385,6 +2379,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2544,7 +2544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2968,12 +2968,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2986,6 +2980,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3435,12 +3435,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3453,6 +3447,12 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mayur Team Member Report
Update team member report for myself
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
+++ b/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\Software2project\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Bhakta\Documents\GitHub\Software2project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="21408" windowHeight="10332" activeTab="1" xr2:uid="{C14DF831-F34F-414D-AAFA-D8324DB30ED1}"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="21408" windowHeight="10332" xr2:uid="{C14DF831-F34F-414D-AAFA-D8324DB30ED1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="67">
   <si>
     <t>Week of</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Sprint 6</t>
-  </si>
-  <si>
-    <t>Mayer Bhakta</t>
   </si>
   <si>
     <t>Andre Manz</t>
@@ -202,6 +199,39 @@
   </si>
   <si>
     <t>Update Documentation</t>
+  </si>
+  <si>
+    <t>Mayur Bhakta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create and update documents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Properly formatting the required documents </t>
+  </si>
+  <si>
+    <t>Update documentations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update documents </t>
+  </si>
+  <si>
+    <t>Update documentations, talk about implementation, and start coding.</t>
+  </si>
+  <si>
+    <t>Created login, account creation, home page screens.</t>
+  </si>
+  <si>
+    <t>Continue creating and updating screens as needed.</t>
+  </si>
+  <si>
+    <t>Assigned task to team members, and worked on new documents for deliverable 2.</t>
+  </si>
+  <si>
+    <t>Clean up GUI, continue updating front end.</t>
+  </si>
+  <si>
+    <t>Some disagreements between members about the use cases</t>
   </si>
 </sst>
 </file>
@@ -567,14 +597,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A726F0A-5F28-4C1C-A552-E596D5063A23}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A271" sqref="A271:D323"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="4" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -587,11 +619,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -600,53 +632,83 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
       <c r="C4" t="s">
         <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="C8" t="s">
         <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -658,12 +720,12 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3"/>
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -672,53 +734,83 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" t="s">
         <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C16" t="s">
         <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C17" t="s">
         <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -730,12 +822,12 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="3"/>
+      <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -744,50 +836,68 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -816,13 +926,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -888,13 +998,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -960,13 +1070,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1011,24 +1121,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1039,7 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6186206B-49DF-4BAF-BCA3-2072C7EB9045}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1061,11 +1171,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -1074,13 +1184,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1088,13 +1198,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1102,13 +1212,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1116,13 +1226,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1151,11 +1261,11 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -1164,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1178,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1192,13 +1302,13 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1206,13 +1316,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1254,13 +1364,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,13 +1436,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1398,13 +1508,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1470,13 +1580,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1521,6 +1631,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
@@ -1530,15 +1649,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1570,11 +1680,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1583,13 +1693,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1597,13 +1707,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1661,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1733,13 +1843,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1805,13 +1915,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1877,13 +1987,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1949,13 +2059,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -2000,6 +2110,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2012,12 +2128,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2027,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63501F0-7A26-4008-89EF-F7F9CD176150}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2050,11 +2160,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -2063,13 +2173,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2077,13 +2187,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2091,13 +2201,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2105,13 +2215,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2119,13 +2229,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2133,13 +2243,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -2152,11 +2262,11 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -2165,13 +2275,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2179,13 +2289,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2193,13 +2303,13 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2207,13 +2317,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2221,13 +2331,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2235,13 +2345,13 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2254,11 +2364,11 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -2267,13 +2377,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2281,7 +2391,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
@@ -2292,7 +2402,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -2303,7 +2413,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -2314,7 +2424,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -2325,7 +2435,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -2354,13 +2464,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2426,13 +2536,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2498,13 +2608,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -2549,6 +2659,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2561,12 +2677,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2577,7 +2687,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D3" sqref="D1:D1048576"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,11 +2708,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -2611,13 +2721,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2625,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -2637,13 +2747,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -2651,13 +2761,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2665,13 +2775,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2679,13 +2789,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2704,11 +2814,11 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -2717,13 +2827,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2731,13 +2841,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
@@ -2745,13 +2855,13 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -2759,13 +2869,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -2773,13 +2883,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -2787,13 +2897,13 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2825,13 +2935,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2913,13 +3023,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3001,13 +3111,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3089,13 +3199,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -3150,6 +3260,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3162,12 +3278,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3193,7 +3303,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -3206,13 +3316,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3278,13 +3388,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3350,13 +3460,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -3422,13 +3532,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3494,13 +3604,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3566,13 +3676,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -3617,6 +3727,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3629,12 +3745,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
myself team member report to sprint 3 2/26/2018
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
+++ b/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arsgate\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carolyn\Documents\GitHub\Software2project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ABEDA5-01BD-4EE1-9343-2F2FD70D1370}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF96CEBC-F518-4F79-97FE-95F8F5CD08C6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="2" xr2:uid="{C14DF831-F34F-414D-AAFA-D8324DB30ED1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="5" xr2:uid="{C14DF831-F34F-414D-AAFA-D8324DB30ED1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="87">
   <si>
     <t>Week of</t>
   </si>
@@ -214,9 +214,6 @@
     <t xml:space="preserve">Update documents </t>
   </si>
   <si>
-    <t>Update documentations, talk about implementation, and start coding.</t>
-  </si>
-  <si>
     <t>Created login, account creation, home page screens.</t>
   </si>
   <si>
@@ -278,6 +275,24 @@
   </si>
   <si>
     <t>Was able to fix java's connection to the mySQL server</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>Created login screen.</t>
+  </si>
+  <si>
+    <t>Week of  2/19/2018</t>
+  </si>
+  <si>
+    <t>Cleaned up GUI  and Create GRL and UCM Models document.</t>
+  </si>
+  <si>
+    <t>how to create GRL and UCM correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> create GRL and UCM correctly</t>
   </si>
 </sst>
 </file>
@@ -321,13 +336,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,37 +659,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A726F0A-5F28-4C1C-A552-E596D5063A23}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -688,7 +703,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -702,7 +717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -716,7 +731,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -730,7 +745,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -744,7 +759,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -758,25 +773,25 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -790,7 +805,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -804,7 +819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -815,10 +830,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,10 +844,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -846,7 +861,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -860,25 +875,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -892,7 +907,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -906,69 +921,69 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -982,7 +997,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -990,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1022,25 +1037,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1054,7 +1069,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -1078,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1086,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1094,25 +1109,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1126,7 +1141,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -1134,7 +1149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1158,7 +1173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1168,9 +1183,516 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6186206B-49DF-4BAF-BCA3-2072C7EB9045}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -1183,519 +1705,12 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6186206B-49DF-4BAF-BCA3-2072C7EB9045}">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>2</v>
-      </c>
-      <c r="C49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1705,37 +1720,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6E39C0-3A30-4150-AA6A-2A04DB3FF51A}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1749,7 +1764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1763,87 +1778,87 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1857,7 +1872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1865,89 +1880,89 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1961,7 +1976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1969,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1977,7 +1992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +2000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +2008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2001,25 +2016,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2033,7 +2048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2041,7 +2056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -2049,7 +2064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2057,7 +2072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2065,7 +2080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2073,25 +2088,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -2105,7 +2120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -2113,7 +2128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -2121,7 +2136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2129,7 +2144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2137,7 +2152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2145,25 +2160,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -2177,7 +2192,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2185,7 +2200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -2193,7 +2208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -2201,7 +2216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2209,7 +2224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2219,6 +2234,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2231,12 +2252,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2247,37 +2262,37 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2305,7 +2320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2319,7 +2334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2333,7 +2348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2347,7 +2362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2361,25 +2376,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2393,7 +2408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2407,7 +2422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -2421,7 +2436,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2435,7 +2450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2449,7 +2464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2463,25 +2478,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2495,7 +2510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2506,7 +2521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -2517,7 +2532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -2528,7 +2543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -2539,7 +2554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2550,25 +2565,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -2582,7 +2597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2590,7 +2605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -2598,7 +2613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2606,7 +2621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -2614,7 +2629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -2622,25 +2637,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -2654,7 +2669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
@@ -2662,7 +2677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -2670,7 +2685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2678,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -2686,7 +2701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -2694,25 +2709,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -2726,7 +2741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
@@ -2734,7 +2749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -2742,7 +2757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -2750,7 +2765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -2758,7 +2773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -2768,6 +2783,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2780,12 +2801,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2795,37 +2810,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0193E54-C821-4268-9DAD-312CE7027412}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2839,7 +2854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2851,7 +2866,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2865,7 +2880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2879,7 +2894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2893,7 +2908,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2907,31 +2922,31 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2945,7 +2960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2959,7 +2974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -2973,7 +2988,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2987,7 +3002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3001,7 +3016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -3015,31 +3030,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -3053,7 +3068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -3063,7 +3078,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -3073,7 +3088,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -3083,7 +3098,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -3093,7 +3108,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -3103,31 +3118,31 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -3141,7 +3156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -3151,7 +3166,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -3161,7 +3176,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -3171,7 +3186,7 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -3181,7 +3196,7 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -3191,31 +3206,31 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -3229,7 +3244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
@@ -3239,7 +3254,7 @@
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -3249,7 +3264,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -3259,7 +3274,7 @@
       </c>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -3269,7 +3284,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -3279,31 +3294,31 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
@@ -3327,7 +3342,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -3337,7 +3352,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -3347,7 +3362,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -3357,7 +3372,7 @@
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -3369,6 +3384,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3381,12 +3402,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3396,31 +3411,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF77B59-FF08-4FBF-8BBC-E87617B2BC46}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3434,65 +3455,95 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3506,65 +3557,95 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -3578,65 +3659,83 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -3650,7 +3749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -3658,7 +3757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -3666,7 +3765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -3674,7 +3773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -3682,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -3690,25 +3789,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -3722,7 +3821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -3730,7 +3829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -3738,7 +3837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -3746,7 +3845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -3754,7 +3853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -3762,25 +3861,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -3794,7 +3893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3802,7 +3901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
@@ -3810,7 +3909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -3818,7 +3917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -3826,7 +3925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -3836,6 +3935,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3848,12 +3953,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Team Member Report Update
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
+++ b/documents/FlyingMongeese_Deliverable_2_Team_Member_Report.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\Software2project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B62018-7C1E-4028-A9BF-D7C5EC91FEEB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mayur" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="107">
   <si>
     <t>Week of</t>
   </si>
@@ -326,6 +325,41 @@
   </si>
   <si>
     <t>Vague instructions on how to fill out the SCMP</t>
+  </si>
+  <si>
+    <t>Using supplimentary .jar files</t>
+  </si>
+  <si>
+    <t>SRS design ignorance</t>
+  </si>
+  <si>
+    <t>Implementing .jar files</t>
+  </si>
+  <si>
+    <t>Research of SRS design/
+requirements</t>
+  </si>
+  <si>
+    <t>Updated Documentation</t>
+  </si>
+  <si>
+    <t>Updated content and syntax of 
+SRS</t>
+  </si>
+  <si>
+    <t>Updated Content and syntax of
+SRS and modified Team
+Member Report</t>
+  </si>
+  <si>
+    <t>Time management due to 
+midterms</t>
+  </si>
+  <si>
+    <t>Content Added to SRS</t>
+  </si>
+  <si>
+    <t>SRS Syntax Fixed</t>
   </si>
 </sst>
 </file>
@@ -856,15 +890,15 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -872,7 +906,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -882,7 +916,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -896,7 +930,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -910,7 +944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -924,7 +958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -938,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -952,7 +986,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -966,13 +1000,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -980,7 +1014,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -990,7 +1024,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1004,7 +1038,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1018,7 +1052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1046,7 +1080,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1060,7 +1094,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -1074,13 +1108,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1122,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -1098,7 +1132,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1146,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -1126,7 +1160,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -1140,7 +1174,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -1154,7 +1188,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -1182,13 +1216,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1230,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1240,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -1220,7 +1254,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -1230,7 +1264,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1274,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -1250,7 +1284,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -1260,7 +1294,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -1270,13 +1304,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1318,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1328,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -1308,7 +1342,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -1318,7 +1352,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -1328,7 +1362,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1338,7 +1372,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -1348,7 +1382,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -1358,13 +1392,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
@@ -1372,7 +1406,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1416,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -1396,7 +1430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -1406,7 +1440,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1450,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1460,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -1436,7 +1470,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -1448,9 +1482,622 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -1463,597 +2110,12 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2067,15 +2129,15 @@
       <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -2083,7 +2145,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -2093,7 +2155,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2107,7 +2169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2121,7 +2183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2137,7 +2199,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2153,7 +2215,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -2169,7 +2231,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -2183,13 +2245,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -2197,7 +2259,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -2207,7 +2269,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -2221,7 +2283,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -2235,7 +2297,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -2251,7 +2313,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -2267,7 +2329,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -2283,7 +2345,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -2299,13 +2361,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -2313,7 +2375,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -2323,7 +2385,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -2337,7 +2399,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2351,7 +2413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -2365,7 +2427,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2379,7 +2441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -2393,7 +2455,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -2407,13 +2469,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -2421,7 +2483,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>0</v>
       </c>
@@ -2431,7 +2493,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -2445,7 +2507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -2455,7 +2517,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -2465,7 +2527,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -2475,7 +2537,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -2485,7 +2547,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -2495,13 +2557,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -2509,7 +2571,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>0</v>
       </c>
@@ -2519,7 +2581,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2533,7 +2595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -2543,7 +2605,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -2553,7 +2615,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -2563,7 +2625,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -2573,7 +2635,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -2583,13 +2645,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>12</v>
       </c>
@@ -2597,7 +2659,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2669,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -2621,7 +2683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -2631,7 +2693,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -2641,7 +2703,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -2651,7 +2713,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -2661,7 +2723,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -2673,6 +2735,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -2685,12 +2753,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2704,16 +2766,16 @@
       <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
@@ -2721,7 +2783,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2793,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2745,7 +2807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2759,7 +2821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2773,7 +2835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2787,7 +2849,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2801,7 +2863,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2815,13 +2877,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -2829,7 +2891,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -2839,7 +2901,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -2853,7 +2915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -2867,7 +2929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -2881,7 +2943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -2895,7 +2957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2909,7 +2971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -2923,13 +2985,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
@@ -2937,7 +2999,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
@@ -2947,7 +3009,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -2961,7 +3023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -2975,7 +3037,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -2989,7 +3051,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3003,7 +3065,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3017,7 +3079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3031,13 +3093,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -3045,7 +3107,7 @@
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>0</v>
       </c>
@@ -3055,7 +3117,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3069,7 +3131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3079,7 +3141,7 @@
       </c>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3089,7 +3151,7 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3099,7 +3161,7 @@
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3109,7 +3171,7 @@
       </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3119,13 +3181,13 @@
       </c>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
@@ -3133,7 +3195,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>0</v>
       </c>
@@ -3143,7 +3205,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3157,7 +3219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3167,7 +3229,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -3177,7 +3239,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3187,7 +3249,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -3197,7 +3259,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -3207,13 +3269,13 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
@@ -3221,7 +3283,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
@@ -3231,7 +3293,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -3245,7 +3307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -3255,7 +3317,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3265,7 +3327,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3275,7 +3337,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -3285,7 +3347,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -3297,6 +3359,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3309,12 +3377,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3328,15 +3390,15 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
@@ -3344,7 +3406,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -3354,7 +3416,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -3368,7 +3430,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -3382,7 +3444,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -3396,7 +3458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3410,7 +3472,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3424,7 +3486,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3438,13 +3500,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -3452,7 +3514,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -3462,7 +3524,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3476,7 +3538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -3490,7 +3552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -3504,7 +3566,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -3518,7 +3580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -3532,7 +3594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -3546,13 +3608,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
@@ -3560,7 +3622,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -3570,7 +3632,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -3584,7 +3646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -3598,7 +3660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -3612,7 +3674,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -3626,7 +3688,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3640,7 +3702,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -3654,13 +3716,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>10</v>
       </c>
@@ -3668,7 +3730,7 @@
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>0</v>
       </c>
@@ -3678,7 +3740,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3692,7 +3754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -3702,7 +3764,7 @@
       </c>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -3712,7 +3774,7 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -3722,7 +3784,7 @@
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -3732,7 +3794,7 @@
       </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -3742,13 +3804,13 @@
       </c>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>11</v>
       </c>
@@ -3756,7 +3818,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>0</v>
       </c>
@@ -3766,7 +3828,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
@@ -3780,7 +3842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3790,7 +3852,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -3800,7 +3862,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -3810,7 +3872,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>5</v>
       </c>
@@ -3820,7 +3882,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
@@ -3830,13 +3892,13 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
         <v>12</v>
       </c>
@@ -3844,7 +3906,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>0</v>
       </c>
@@ -3854,7 +3916,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>1</v>
       </c>
@@ -3868,7 +3930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -3878,7 +3940,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3888,7 +3950,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -3898,7 +3960,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>5</v>
       </c>
@@ -3908,7 +3970,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>6</v>
       </c>
@@ -3920,6 +3982,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -3932,12 +4000,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3948,19 +4010,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
@@ -3968,7 +4030,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -3978,7 +4040,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -3992,7 +4054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4006,7 +4068,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -4020,7 +4082,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -4034,7 +4096,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -4048,7 +4110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -4062,13 +4124,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -4076,7 +4138,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -4086,7 +4148,7 @@
       </c>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -4100,7 +4162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -4114,7 +4176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -4128,7 +4190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4142,7 +4204,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -4156,7 +4218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -4170,13 +4232,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -4184,7 +4246,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
@@ -4194,7 +4256,7 @@
       </c>
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
@@ -4208,7 +4270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -4222,7 +4284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
@@ -4236,7 +4298,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -4250,7 +4312,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -4264,7 +4326,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -4278,13 +4340,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -4292,7 +4354,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>18</v>
       </c>
@@ -4302,7 +4364,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>1</v>
       </c>
@@ -4316,7 +4378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -4326,7 +4388,7 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
@@ -4336,7 +4398,7 @@
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -4346,7 +4408,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -4356,7 +4418,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>6</v>
       </c>
@@ -4366,13 +4428,13 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -4380,7 +4442,7 @@
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>18</v>
       </c>
@@ -4390,7 +4452,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>1</v>
       </c>
@@ -4404,7 +4466,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -4414,7 +4476,7 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>3</v>
       </c>
@@ -4424,7 +4486,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -4434,7 +4496,7 @@
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -4444,7 +4506,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -4454,13 +4516,13 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>11</v>
       </c>
@@ -4468,7 +4530,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>18</v>
       </c>
@@ -4478,7 +4540,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>1</v>
       </c>
@@ -4492,7 +4554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -4502,7 +4564,7 @@
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4512,7 +4574,7 @@
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -4522,7 +4584,7 @@
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>5</v>
       </c>
@@ -4532,7 +4594,7 @@
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>6</v>
       </c>
@@ -4544,6 +4606,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
@@ -4556,12 +4624,6 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>